<commit_message>
finished cleaning up data in R
</commit_message>
<xml_diff>
--- a/Data/Caterpillars/RawData/Caterpillar Predation data.xlsx
+++ b/Data/Caterpillars/RawData/Caterpillar Predation data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brittanycavazos\Documents\EEB_590\ClayCaterpillarProject\Data\Caterpillars\RawData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brittanycavazos\Documents\EEB_590\ClayCaterpillarProject\bcavazos\Data\Caterpillars\RawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11232" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11234" uniqueCount="176">
   <si>
     <t>Island</t>
   </si>
@@ -499,9 +499,6 @@
     <t>mislabeled - #119 was upredated (possibly #121 is true ID) - BRC - 9/20/16</t>
   </si>
   <si>
-    <t>mislabeled - #14 was unpredated - bRC 9/20/16</t>
-  </si>
-  <si>
     <t>mislabeled - #68 was unpredated - BRC 9/20/16</t>
   </si>
   <si>
@@ -553,7 +550,13 @@
     <t>each predation event assigned a Type based on physical markings. See H8:I24</t>
   </si>
   <si>
-    <t>Update: BRC 9/26/16 - changed number column in predationID to text type instead of numeric in hopes it will fix the read_exel problem</t>
+    <t>mislabeled - #14 was unpredated - BRC 9/20/16</t>
+  </si>
+  <si>
+    <t>Update: BRC 9/30/16 - link to predation photos https://www.dropbox.com/sh/p7rgtti4t2qtdxw/AACGi4TQUiR7DkgAh3cd07XYa?dl=0 - not all photos are labeled, making it impossible to verify all predation markings; D11 changed to 43a to match with that in caterpillar data - this number was reassigned when there were 2 43's in raw data, one predated and one unpredated</t>
+  </si>
+  <si>
+    <t>Update: BRC 9/26/16 - changed number column in predationID to text type instead of numeric in hopes it will fix the read_excel problem</t>
   </si>
 </sst>
 </file>
@@ -657,7 +660,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -665,6 +668,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -677,8 +683,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1041,8 +1045,8 @@
   <dimension ref="A1:I1651"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A636" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I148" sqref="I148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1073,7 +1077,7 @@
         <v>70</v>
       </c>
       <c r="H1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I1" t="s">
         <v>97</v>
@@ -44085,12 +44089,12 @@
   <dimension ref="A1:H295"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11.19921875" style="12"/>
+    <col min="4" max="4" width="11.19921875" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -44103,7 +44107,7 @@
       <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -44123,13 +44127,13 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="8">
         <v>68</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="7"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -44141,13 +44145,13 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="8">
         <v>58</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -44159,13 +44163,13 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="8">
         <v>51</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="9" t="s">
         <v>154</v>
       </c>
     </row>
@@ -44179,7 +44183,7 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="8">
         <v>18</v>
       </c>
       <c r="E5" t="s">
@@ -44196,7 +44200,7 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="8">
         <v>147</v>
       </c>
       <c r="E6" t="s">
@@ -44213,12 +44217,13 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="8">
         <v>141</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
       </c>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -44230,7 +44235,7 @@
       <c r="C8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="8">
         <v>130</v>
       </c>
       <c r="E8" t="s">
@@ -44247,7 +44252,7 @@
       <c r="C9" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="8">
         <v>73</v>
       </c>
       <c r="E9" t="s">
@@ -44264,7 +44269,7 @@
       <c r="C10" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="8">
         <v>70</v>
       </c>
       <c r="E10" t="s">
@@ -44281,8 +44286,8 @@
       <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="12">
-        <v>43</v>
+      <c r="D11" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
@@ -44298,7 +44303,7 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="8">
         <v>38</v>
       </c>
       <c r="E12" t="s">
@@ -44315,7 +44320,7 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="8">
         <v>36</v>
       </c>
       <c r="E13" t="s">
@@ -44332,7 +44337,7 @@
       <c r="C14" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="8">
         <v>37</v>
       </c>
       <c r="E14" t="s">
@@ -44349,7 +44354,7 @@
       <c r="C15" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="8">
         <v>130</v>
       </c>
       <c r="E15" t="s">
@@ -44366,7 +44371,7 @@
       <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="8">
         <v>125</v>
       </c>
       <c r="E16" t="s">
@@ -44383,7 +44388,7 @@
       <c r="C17" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="8">
         <v>106</v>
       </c>
       <c r="E17" t="s">
@@ -44400,7 +44405,7 @@
       <c r="C18" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="8">
         <v>55</v>
       </c>
       <c r="E18" t="s">
@@ -44417,7 +44422,7 @@
       <c r="C19" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="8">
         <v>79</v>
       </c>
       <c r="E19" t="s">
@@ -44434,7 +44439,7 @@
       <c r="C20" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="8">
         <v>85</v>
       </c>
       <c r="E20" t="s">
@@ -44451,7 +44456,7 @@
       <c r="C21" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="8">
         <v>104</v>
       </c>
       <c r="E21" t="s">
@@ -44468,7 +44473,7 @@
       <c r="C22" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="8">
         <v>111</v>
       </c>
       <c r="E22" t="s">
@@ -44485,7 +44490,7 @@
       <c r="C23" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="8">
         <v>118</v>
       </c>
       <c r="E23" t="s">
@@ -44502,7 +44507,7 @@
       <c r="C24" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="8">
         <v>119</v>
       </c>
       <c r="E24" t="s">
@@ -44519,7 +44524,7 @@
       <c r="C25" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="8">
         <v>145</v>
       </c>
       <c r="E25" t="s">
@@ -44536,7 +44541,7 @@
       <c r="C26" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="8">
         <v>141</v>
       </c>
       <c r="E26" t="s">
@@ -44553,7 +44558,7 @@
       <c r="C27" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D27" s="8">
         <v>139</v>
       </c>
       <c r="E27" t="s">
@@ -44570,7 +44575,7 @@
       <c r="C28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28" s="8">
         <v>135</v>
       </c>
       <c r="E28" t="s">
@@ -44587,7 +44592,7 @@
       <c r="C29" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29" s="8">
         <v>117</v>
       </c>
       <c r="E29" t="s">
@@ -44604,7 +44609,7 @@
       <c r="C30" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="8">
         <v>115</v>
       </c>
       <c r="E30" t="s">
@@ -44621,7 +44626,7 @@
       <c r="C31" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="12">
+      <c r="D31" s="8">
         <v>102</v>
       </c>
       <c r="E31" t="s">
@@ -44638,7 +44643,7 @@
       <c r="C32" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="8">
         <v>89</v>
       </c>
       <c r="E32" t="s">
@@ -44655,7 +44660,7 @@
       <c r="C33" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="12">
+      <c r="D33" s="8">
         <v>79</v>
       </c>
       <c r="E33" t="s">
@@ -44672,7 +44677,7 @@
       <c r="C34" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="12">
+      <c r="D34" s="8">
         <v>52</v>
       </c>
       <c r="E34" t="s">
@@ -44689,7 +44694,7 @@
       <c r="C35" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="12">
+      <c r="D35" s="8">
         <v>105</v>
       </c>
       <c r="E35" t="s">
@@ -44706,7 +44711,7 @@
       <c r="C36" t="s">
         <v>13</v>
       </c>
-      <c r="D36" s="12">
+      <c r="D36" s="8">
         <v>103</v>
       </c>
       <c r="E36" t="s">
@@ -44723,7 +44728,7 @@
       <c r="C37" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="12">
+      <c r="D37" s="8">
         <v>41</v>
       </c>
       <c r="E37" t="s">
@@ -44740,7 +44745,7 @@
       <c r="C38" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="12">
+      <c r="D38" s="8">
         <v>40</v>
       </c>
       <c r="E38" t="s">
@@ -44757,7 +44762,7 @@
       <c r="C39" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="12">
+      <c r="D39" s="8">
         <v>36</v>
       </c>
       <c r="E39" t="s">
@@ -44774,7 +44779,7 @@
       <c r="C40" t="s">
         <v>13</v>
       </c>
-      <c r="D40" s="12">
+      <c r="D40" s="8">
         <v>30</v>
       </c>
       <c r="E40" t="s">
@@ -44791,7 +44796,7 @@
       <c r="C41" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="12">
+      <c r="D41" s="8">
         <v>26</v>
       </c>
       <c r="E41" t="s">
@@ -44808,7 +44813,7 @@
       <c r="C42" t="s">
         <v>13</v>
       </c>
-      <c r="D42" s="12">
+      <c r="D42" s="8">
         <v>25</v>
       </c>
       <c r="E42" t="s">
@@ -44825,7 +44830,7 @@
       <c r="C43" t="s">
         <v>13</v>
       </c>
-      <c r="D43" s="12">
+      <c r="D43" s="8">
         <v>22</v>
       </c>
       <c r="E43" t="s">
@@ -44842,7 +44847,7 @@
       <c r="C44" t="s">
         <v>13</v>
       </c>
-      <c r="D44" s="12">
+      <c r="D44" s="8">
         <v>18</v>
       </c>
       <c r="E44" t="s">
@@ -44859,7 +44864,7 @@
       <c r="C45" t="s">
         <v>13</v>
       </c>
-      <c r="D45" s="12">
+      <c r="D45" s="8">
         <v>17</v>
       </c>
       <c r="E45" t="s">
@@ -44876,7 +44881,7 @@
       <c r="C46" t="s">
         <v>13</v>
       </c>
-      <c r="D46" s="12">
+      <c r="D46" s="8">
         <v>8</v>
       </c>
       <c r="E46" t="s">
@@ -44893,7 +44898,7 @@
       <c r="C47" t="s">
         <v>51</v>
       </c>
-      <c r="D47" s="12">
+      <c r="D47" s="8">
         <v>133</v>
       </c>
       <c r="E47" t="s">
@@ -44910,7 +44915,7 @@
       <c r="C48" t="s">
         <v>51</v>
       </c>
-      <c r="D48" s="12">
+      <c r="D48" s="8">
         <v>130</v>
       </c>
       <c r="E48" t="s">
@@ -44927,7 +44932,7 @@
       <c r="C49" t="s">
         <v>51</v>
       </c>
-      <c r="D49" s="12">
+      <c r="D49" s="8">
         <v>117</v>
       </c>
       <c r="E49" t="s">
@@ -44944,7 +44949,7 @@
       <c r="C50" t="s">
         <v>51</v>
       </c>
-      <c r="D50" s="12">
+      <c r="D50" s="8">
         <v>107</v>
       </c>
       <c r="E50" t="s">
@@ -44961,7 +44966,7 @@
       <c r="C51" t="s">
         <v>51</v>
       </c>
-      <c r="D51" s="12">
+      <c r="D51" s="8">
         <v>101</v>
       </c>
       <c r="E51" t="s">
@@ -44978,7 +44983,7 @@
       <c r="C52" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="12">
+      <c r="D52" s="8">
         <v>80</v>
       </c>
       <c r="E52" t="s">
@@ -44995,7 +45000,7 @@
       <c r="C53" t="s">
         <v>51</v>
       </c>
-      <c r="D53" s="12">
+      <c r="D53" s="8">
         <v>74</v>
       </c>
       <c r="E53" t="s">
@@ -45012,7 +45017,7 @@
       <c r="C54" t="s">
         <v>51</v>
       </c>
-      <c r="D54" s="12">
+      <c r="D54" s="8">
         <v>33</v>
       </c>
       <c r="E54" t="s">
@@ -45029,7 +45034,7 @@
       <c r="C55" t="s">
         <v>51</v>
       </c>
-      <c r="D55" s="12">
+      <c r="D55" s="8">
         <v>32</v>
       </c>
       <c r="E55" t="s">
@@ -45046,7 +45051,7 @@
       <c r="C56" t="s">
         <v>51</v>
       </c>
-      <c r="D56" s="12">
+      <c r="D56" s="8">
         <v>31</v>
       </c>
       <c r="E56" t="s">
@@ -45063,7 +45068,7 @@
       <c r="C57" t="s">
         <v>51</v>
       </c>
-      <c r="D57" s="12">
+      <c r="D57" s="8">
         <v>27</v>
       </c>
       <c r="E57" t="s">
@@ -45080,7 +45085,7 @@
       <c r="C58" t="s">
         <v>51</v>
       </c>
-      <c r="D58" s="12">
+      <c r="D58" s="8">
         <v>25</v>
       </c>
       <c r="E58" t="s">
@@ -45097,7 +45102,7 @@
       <c r="C59" t="s">
         <v>51</v>
       </c>
-      <c r="D59" s="12">
+      <c r="D59" s="8">
         <v>17</v>
       </c>
       <c r="E59" t="s">
@@ -45114,7 +45119,7 @@
       <c r="C60" t="s">
         <v>51</v>
       </c>
-      <c r="D60" s="12">
+      <c r="D60" s="8">
         <v>15</v>
       </c>
       <c r="E60" t="s">
@@ -45131,7 +45136,7 @@
       <c r="C61" t="s">
         <v>51</v>
       </c>
-      <c r="D61" s="12">
+      <c r="D61" s="8">
         <v>13</v>
       </c>
       <c r="E61" t="s">
@@ -45148,7 +45153,7 @@
       <c r="C62" t="s">
         <v>51</v>
       </c>
-      <c r="D62" s="12">
+      <c r="D62" s="8">
         <v>11</v>
       </c>
       <c r="E62" t="s">
@@ -45165,7 +45170,7 @@
       <c r="C63" t="s">
         <v>51</v>
       </c>
-      <c r="D63" s="12">
+      <c r="D63" s="8">
         <v>5</v>
       </c>
       <c r="E63" t="s">
@@ -45182,7 +45187,7 @@
       <c r="C64" t="s">
         <v>28</v>
       </c>
-      <c r="D64" s="12">
+      <c r="D64" s="8">
         <v>134</v>
       </c>
       <c r="E64" t="s">
@@ -45199,7 +45204,7 @@
       <c r="C65" t="s">
         <v>28</v>
       </c>
-      <c r="D65" s="12">
+      <c r="D65" s="8">
         <v>126</v>
       </c>
       <c r="E65" t="s">
@@ -45216,7 +45221,7 @@
       <c r="C66" t="s">
         <v>28</v>
       </c>
-      <c r="D66" s="12">
+      <c r="D66" s="8">
         <v>119</v>
       </c>
       <c r="E66" t="s">
@@ -45236,7 +45241,7 @@
       <c r="C67" t="s">
         <v>28</v>
       </c>
-      <c r="D67" s="12">
+      <c r="D67" s="8">
         <v>106</v>
       </c>
       <c r="E67" t="s">
@@ -45253,7 +45258,7 @@
       <c r="C68" t="s">
         <v>28</v>
       </c>
-      <c r="D68" s="12">
+      <c r="D68" s="8">
         <v>104</v>
       </c>
       <c r="E68" t="s">
@@ -45270,7 +45275,7 @@
       <c r="C69" t="s">
         <v>28</v>
       </c>
-      <c r="D69" s="12">
+      <c r="D69" s="8">
         <v>99</v>
       </c>
       <c r="E69" t="s">
@@ -45287,7 +45292,7 @@
       <c r="C70" t="s">
         <v>28</v>
       </c>
-      <c r="D70" s="12">
+      <c r="D70" s="8">
         <v>87</v>
       </c>
       <c r="E70" t="s">
@@ -45304,7 +45309,7 @@
       <c r="C71" t="s">
         <v>28</v>
       </c>
-      <c r="D71" s="12">
+      <c r="D71" s="8">
         <v>86</v>
       </c>
       <c r="E71" t="s">
@@ -45321,7 +45326,7 @@
       <c r="C72" t="s">
         <v>28</v>
       </c>
-      <c r="D72" s="12">
+      <c r="D72" s="8">
         <v>79</v>
       </c>
       <c r="E72" t="s">
@@ -45338,7 +45343,7 @@
       <c r="C73" t="s">
         <v>28</v>
       </c>
-      <c r="D73" s="12">
+      <c r="D73" s="8">
         <v>77</v>
       </c>
       <c r="E73" t="s">
@@ -45355,7 +45360,7 @@
       <c r="C74" t="s">
         <v>28</v>
       </c>
-      <c r="D74" s="12">
+      <c r="D74" s="8">
         <v>70</v>
       </c>
       <c r="E74" t="s">
@@ -45372,7 +45377,7 @@
       <c r="C75" t="s">
         <v>28</v>
       </c>
-      <c r="D75" s="12">
+      <c r="D75" s="8">
         <v>67</v>
       </c>
       <c r="E75" t="s">
@@ -45389,7 +45394,7 @@
       <c r="C76" t="s">
         <v>28</v>
       </c>
-      <c r="D76" s="12">
+      <c r="D76" s="8">
         <v>54</v>
       </c>
       <c r="E76" t="s">
@@ -45406,7 +45411,7 @@
       <c r="C77" t="s">
         <v>28</v>
       </c>
-      <c r="D77" s="12">
+      <c r="D77" s="8">
         <v>43</v>
       </c>
       <c r="E77" t="s">
@@ -45423,7 +45428,7 @@
       <c r="C78" t="s">
         <v>28</v>
       </c>
-      <c r="D78" s="12">
+      <c r="D78" s="8">
         <v>37</v>
       </c>
       <c r="E78" t="s">
@@ -45440,7 +45445,7 @@
       <c r="C79" t="s">
         <v>28</v>
       </c>
-      <c r="D79" s="12">
+      <c r="D79" s="8">
         <v>36</v>
       </c>
       <c r="E79" t="s">
@@ -45457,7 +45462,7 @@
       <c r="C80" t="s">
         <v>28</v>
       </c>
-      <c r="D80" s="12">
+      <c r="D80" s="8">
         <v>35</v>
       </c>
       <c r="E80" t="s">
@@ -45474,7 +45479,7 @@
       <c r="C81" t="s">
         <v>28</v>
       </c>
-      <c r="D81" s="12">
+      <c r="D81" s="8">
         <v>29</v>
       </c>
       <c r="E81" t="s">
@@ -45491,7 +45496,7 @@
       <c r="C82" t="s">
         <v>28</v>
       </c>
-      <c r="D82" s="12">
+      <c r="D82" s="8">
         <v>27</v>
       </c>
       <c r="E82" t="s">
@@ -45508,7 +45513,7 @@
       <c r="C83" t="s">
         <v>28</v>
       </c>
-      <c r="D83" s="12">
+      <c r="D83" s="8">
         <v>25</v>
       </c>
       <c r="E83" t="s">
@@ -45525,7 +45530,7 @@
       <c r="C84" t="s">
         <v>28</v>
       </c>
-      <c r="D84" s="12">
+      <c r="D84" s="8">
         <v>21</v>
       </c>
       <c r="E84" t="s">
@@ -45542,7 +45547,7 @@
       <c r="C85" t="s">
         <v>28</v>
       </c>
-      <c r="D85" s="12">
+      <c r="D85" s="8">
         <v>20</v>
       </c>
       <c r="E85" t="s">
@@ -45559,7 +45564,7 @@
       <c r="C86" t="s">
         <v>28</v>
       </c>
-      <c r="D86" s="12">
+      <c r="D86" s="8">
         <v>15</v>
       </c>
       <c r="E86" t="s">
@@ -45576,7 +45581,7 @@
       <c r="C87" t="s">
         <v>28</v>
       </c>
-      <c r="D87" s="12">
+      <c r="D87" s="8">
         <v>14</v>
       </c>
       <c r="E87" t="s">
@@ -45593,7 +45598,7 @@
       <c r="C88" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="12">
+      <c r="D88" s="8">
         <v>11</v>
       </c>
       <c r="E88" t="s">
@@ -45610,7 +45615,7 @@
       <c r="C89" t="s">
         <v>28</v>
       </c>
-      <c r="D89" s="12">
+      <c r="D89" s="8">
         <v>8</v>
       </c>
       <c r="E89" t="s">
@@ -45627,7 +45632,7 @@
       <c r="C90" t="s">
         <v>28</v>
       </c>
-      <c r="D90" s="12">
+      <c r="D90" s="8">
         <v>2</v>
       </c>
       <c r="E90" t="s">
@@ -45644,7 +45649,7 @@
       <c r="C91" t="s">
         <v>28</v>
       </c>
-      <c r="D91" s="12">
+      <c r="D91" s="8">
         <v>1</v>
       </c>
       <c r="E91" t="s">
@@ -45661,7 +45666,7 @@
       <c r="C92" t="s">
         <v>35</v>
       </c>
-      <c r="D92" s="12">
+      <c r="D92" s="8">
         <v>152</v>
       </c>
       <c r="E92" t="s">
@@ -45678,7 +45683,7 @@
       <c r="C93" t="s">
         <v>35</v>
       </c>
-      <c r="D93" s="12">
+      <c r="D93" s="8">
         <v>115</v>
       </c>
       <c r="E93" t="s">
@@ -45695,7 +45700,7 @@
       <c r="C94" t="s">
         <v>35</v>
       </c>
-      <c r="D94" s="12">
+      <c r="D94" s="8">
         <v>112</v>
       </c>
       <c r="E94" t="s">
@@ -45712,7 +45717,7 @@
       <c r="C95" t="s">
         <v>35</v>
       </c>
-      <c r="D95" s="12">
+      <c r="D95" s="8">
         <v>100</v>
       </c>
       <c r="E95" t="s">
@@ -45729,7 +45734,7 @@
       <c r="C96" t="s">
         <v>35</v>
       </c>
-      <c r="D96" s="12">
+      <c r="D96" s="8">
         <v>98</v>
       </c>
       <c r="E96" t="s">
@@ -45746,7 +45751,7 @@
       <c r="C97" t="s">
         <v>35</v>
       </c>
-      <c r="D97" s="12">
+      <c r="D97" s="8">
         <v>97</v>
       </c>
       <c r="E97" t="s">
@@ -45763,7 +45768,7 @@
       <c r="C98" t="s">
         <v>35</v>
       </c>
-      <c r="D98" s="12">
+      <c r="D98" s="8">
         <v>96</v>
       </c>
       <c r="E98" t="s">
@@ -45780,7 +45785,7 @@
       <c r="C99" t="s">
         <v>35</v>
       </c>
-      <c r="D99" s="12">
+      <c r="D99" s="8">
         <v>94</v>
       </c>
       <c r="E99" t="s">
@@ -45797,7 +45802,7 @@
       <c r="C100" t="s">
         <v>35</v>
       </c>
-      <c r="D100" s="12">
+      <c r="D100" s="8">
         <v>87</v>
       </c>
       <c r="E100" t="s">
@@ -45814,7 +45819,7 @@
       <c r="C101" t="s">
         <v>35</v>
       </c>
-      <c r="D101" s="12">
+      <c r="D101" s="8">
         <v>78</v>
       </c>
       <c r="E101" t="s">
@@ -45831,7 +45836,7 @@
       <c r="C102" t="s">
         <v>35</v>
       </c>
-      <c r="D102" s="12">
+      <c r="D102" s="8">
         <v>77</v>
       </c>
       <c r="E102" t="s">
@@ -45848,7 +45853,7 @@
       <c r="C103" t="s">
         <v>35</v>
       </c>
-      <c r="D103" s="12">
+      <c r="D103" s="8">
         <v>64</v>
       </c>
       <c r="E103" t="s">
@@ -45865,7 +45870,7 @@
       <c r="C104" t="s">
         <v>35</v>
       </c>
-      <c r="D104" s="12">
+      <c r="D104" s="8">
         <v>62</v>
       </c>
       <c r="E104" t="s">
@@ -45882,7 +45887,7 @@
       <c r="C105" t="s">
         <v>35</v>
       </c>
-      <c r="D105" s="12">
+      <c r="D105" s="8">
         <v>61</v>
       </c>
       <c r="E105" t="s">
@@ -45899,7 +45904,7 @@
       <c r="C106" t="s">
         <v>35</v>
       </c>
-      <c r="D106" s="12">
+      <c r="D106" s="8">
         <v>45</v>
       </c>
       <c r="E106" t="s">
@@ -45916,7 +45921,7 @@
       <c r="C107" t="s">
         <v>35</v>
       </c>
-      <c r="D107" s="12">
+      <c r="D107" s="8">
         <v>57</v>
       </c>
       <c r="E107" t="s">
@@ -45933,7 +45938,7 @@
       <c r="C108" t="s">
         <v>35</v>
       </c>
-      <c r="D108" s="12">
+      <c r="D108" s="8">
         <v>51</v>
       </c>
       <c r="E108" t="s">
@@ -45950,7 +45955,7 @@
       <c r="C109" t="s">
         <v>35</v>
       </c>
-      <c r="D109" s="12">
+      <c r="D109" s="8">
         <v>48</v>
       </c>
       <c r="E109" t="s">
@@ -45967,7 +45972,7 @@
       <c r="C110" t="s">
         <v>35</v>
       </c>
-      <c r="D110" s="12">
+      <c r="D110" s="8">
         <v>43</v>
       </c>
       <c r="E110" t="s">
@@ -45984,7 +45989,7 @@
       <c r="C111" t="s">
         <v>35</v>
       </c>
-      <c r="D111" s="12">
+      <c r="D111" s="8">
         <v>41</v>
       </c>
       <c r="E111" t="s">
@@ -46001,7 +46006,7 @@
       <c r="C112" t="s">
         <v>35</v>
       </c>
-      <c r="D112" s="12">
+      <c r="D112" s="8">
         <v>40</v>
       </c>
       <c r="E112" t="s">
@@ -46018,7 +46023,7 @@
       <c r="C113" t="s">
         <v>35</v>
       </c>
-      <c r="D113" s="12">
+      <c r="D113" s="8">
         <v>21</v>
       </c>
       <c r="E113" t="s">
@@ -46035,7 +46040,7 @@
       <c r="C114" t="s">
         <v>35</v>
       </c>
-      <c r="D114" s="12">
+      <c r="D114" s="8">
         <v>18</v>
       </c>
       <c r="E114" t="s">
@@ -46052,7 +46057,7 @@
       <c r="C115" t="s">
         <v>35</v>
       </c>
-      <c r="D115" s="12">
+      <c r="D115" s="8">
         <v>16</v>
       </c>
       <c r="E115" t="s">
@@ -46069,7 +46074,7 @@
       <c r="C116" t="s">
         <v>35</v>
       </c>
-      <c r="D116" s="12">
+      <c r="D116" s="8">
         <v>6</v>
       </c>
       <c r="E116" t="s">
@@ -46086,7 +46091,7 @@
       <c r="C117" t="s">
         <v>40</v>
       </c>
-      <c r="D117" s="12">
+      <c r="D117" s="8">
         <v>147</v>
       </c>
       <c r="E117" t="s">
@@ -46103,7 +46108,7 @@
       <c r="C118" t="s">
         <v>40</v>
       </c>
-      <c r="D118" s="12">
+      <c r="D118" s="8">
         <v>145</v>
       </c>
       <c r="E118" t="s">
@@ -46120,7 +46125,7 @@
       <c r="C119" t="s">
         <v>40</v>
       </c>
-      <c r="D119" s="12">
+      <c r="D119" s="8">
         <v>144</v>
       </c>
       <c r="E119" t="s">
@@ -46137,7 +46142,7 @@
       <c r="C120" t="s">
         <v>40</v>
       </c>
-      <c r="D120" s="12">
+      <c r="D120" s="8">
         <v>143</v>
       </c>
       <c r="E120" t="s">
@@ -46154,7 +46159,7 @@
       <c r="C121" t="s">
         <v>40</v>
       </c>
-      <c r="D121" s="12">
+      <c r="D121" s="8">
         <v>142</v>
       </c>
       <c r="E121" t="s">
@@ -46171,7 +46176,7 @@
       <c r="C122" t="s">
         <v>40</v>
       </c>
-      <c r="D122" s="12">
+      <c r="D122" s="8">
         <v>140</v>
       </c>
       <c r="E122" t="s">
@@ -46188,7 +46193,7 @@
       <c r="C123" t="s">
         <v>40</v>
       </c>
-      <c r="D123" s="12">
+      <c r="D123" s="8">
         <v>138</v>
       </c>
       <c r="E123" t="s">
@@ -46205,7 +46210,7 @@
       <c r="C124" t="s">
         <v>40</v>
       </c>
-      <c r="D124" s="12">
+      <c r="D124" s="8">
         <v>132</v>
       </c>
       <c r="E124" t="s">
@@ -46222,7 +46227,7 @@
       <c r="C125" t="s">
         <v>40</v>
       </c>
-      <c r="D125" s="12">
+      <c r="D125" s="8">
         <v>131</v>
       </c>
       <c r="E125" t="s">
@@ -46239,7 +46244,7 @@
       <c r="C126" t="s">
         <v>40</v>
       </c>
-      <c r="D126" s="12">
+      <c r="D126" s="8">
         <v>129</v>
       </c>
       <c r="E126" t="s">
@@ -46256,7 +46261,7 @@
       <c r="C127" t="s">
         <v>40</v>
       </c>
-      <c r="D127" s="12">
+      <c r="D127" s="8">
         <v>128</v>
       </c>
       <c r="E127" t="s">
@@ -46273,7 +46278,7 @@
       <c r="C128" t="s">
         <v>40</v>
       </c>
-      <c r="D128" s="12">
+      <c r="D128" s="8">
         <v>127</v>
       </c>
       <c r="E128" t="s">
@@ -46290,7 +46295,7 @@
       <c r="C129" t="s">
         <v>40</v>
       </c>
-      <c r="D129" s="12">
+      <c r="D129" s="8">
         <v>125</v>
       </c>
       <c r="E129" t="s">
@@ -46307,7 +46312,7 @@
       <c r="C130" t="s">
         <v>40</v>
       </c>
-      <c r="D130" s="12">
+      <c r="D130" s="8">
         <v>123</v>
       </c>
       <c r="E130" t="s">
@@ -46324,7 +46329,7 @@
       <c r="C131" t="s">
         <v>40</v>
       </c>
-      <c r="D131" s="12">
+      <c r="D131" s="8">
         <v>114</v>
       </c>
       <c r="E131" t="s">
@@ -46341,7 +46346,7 @@
       <c r="C132" t="s">
         <v>40</v>
       </c>
-      <c r="D132" s="12">
+      <c r="D132" s="8">
         <v>113</v>
       </c>
       <c r="E132" t="s">
@@ -46358,7 +46363,7 @@
       <c r="C133" t="s">
         <v>40</v>
       </c>
-      <c r="D133" s="12">
+      <c r="D133" s="8">
         <v>111</v>
       </c>
       <c r="E133" t="s">
@@ -46375,7 +46380,7 @@
       <c r="C134" t="s">
         <v>40</v>
       </c>
-      <c r="D134" s="12">
+      <c r="D134" s="8">
         <v>110</v>
       </c>
       <c r="E134" t="s">
@@ -46392,7 +46397,7 @@
       <c r="C135" t="s">
         <v>40</v>
       </c>
-      <c r="D135" s="12">
+      <c r="D135" s="8">
         <v>105</v>
       </c>
       <c r="E135" t="s">
@@ -46409,7 +46414,7 @@
       <c r="C136" t="s">
         <v>40</v>
       </c>
-      <c r="D136" s="12">
+      <c r="D136" s="8">
         <v>104</v>
       </c>
       <c r="E136" t="s">
@@ -46426,7 +46431,7 @@
       <c r="C137" t="s">
         <v>40</v>
       </c>
-      <c r="D137" s="12">
+      <c r="D137" s="8">
         <v>103</v>
       </c>
       <c r="E137" t="s">
@@ -46443,7 +46448,7 @@
       <c r="C138" t="s">
         <v>40</v>
       </c>
-      <c r="D138" s="12">
+      <c r="D138" s="8">
         <v>101</v>
       </c>
       <c r="E138" t="s">
@@ -46460,7 +46465,7 @@
       <c r="C139" t="s">
         <v>40</v>
       </c>
-      <c r="D139" s="12">
+      <c r="D139" s="8">
         <v>98</v>
       </c>
       <c r="E139" t="s">
@@ -46477,7 +46482,7 @@
       <c r="C140" t="s">
         <v>40</v>
       </c>
-      <c r="D140" s="12">
+      <c r="D140" s="8">
         <v>96</v>
       </c>
       <c r="E140" t="s">
@@ -46494,7 +46499,7 @@
       <c r="C141" t="s">
         <v>40</v>
       </c>
-      <c r="D141" s="12">
+      <c r="D141" s="8">
         <v>94</v>
       </c>
       <c r="E141" t="s">
@@ -46511,7 +46516,7 @@
       <c r="C142" t="s">
         <v>40</v>
       </c>
-      <c r="D142" s="12">
+      <c r="D142" s="8">
         <v>93</v>
       </c>
       <c r="E142" t="s">
@@ -46528,7 +46533,7 @@
       <c r="C143" t="s">
         <v>40</v>
       </c>
-      <c r="D143" s="12">
+      <c r="D143" s="8">
         <v>90</v>
       </c>
       <c r="E143" t="s">
@@ -46545,7 +46550,7 @@
       <c r="C144" t="s">
         <v>40</v>
       </c>
-      <c r="D144" s="12">
+      <c r="D144" s="8">
         <v>87</v>
       </c>
       <c r="E144" t="s">
@@ -46562,7 +46567,7 @@
       <c r="C145" t="s">
         <v>40</v>
       </c>
-      <c r="D145" s="12">
+      <c r="D145" s="8">
         <v>86</v>
       </c>
       <c r="E145" t="s">
@@ -46579,7 +46584,7 @@
       <c r="C146" t="s">
         <v>40</v>
       </c>
-      <c r="D146" s="12">
+      <c r="D146" s="8">
         <v>83</v>
       </c>
       <c r="E146" t="s">
@@ -46596,7 +46601,7 @@
       <c r="C147" t="s">
         <v>40</v>
       </c>
-      <c r="D147" s="12">
+      <c r="D147" s="8">
         <v>80</v>
       </c>
       <c r="E147" t="s">
@@ -46613,7 +46618,7 @@
       <c r="C148" t="s">
         <v>40</v>
       </c>
-      <c r="D148" s="12">
+      <c r="D148" s="8">
         <v>79</v>
       </c>
       <c r="E148" t="s">
@@ -46630,7 +46635,7 @@
       <c r="C149" t="s">
         <v>40</v>
       </c>
-      <c r="D149" s="12">
+      <c r="D149" s="8">
         <v>78</v>
       </c>
       <c r="E149" t="s">
@@ -46647,7 +46652,7 @@
       <c r="C150" t="s">
         <v>40</v>
       </c>
-      <c r="D150" s="12">
+      <c r="D150" s="8">
         <v>75</v>
       </c>
       <c r="E150" t="s">
@@ -46664,7 +46669,7 @@
       <c r="C151" t="s">
         <v>40</v>
       </c>
-      <c r="D151" s="12" t="s">
+      <c r="D151" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E151" t="s">
@@ -46681,7 +46686,7 @@
       <c r="C152" t="s">
         <v>40</v>
       </c>
-      <c r="D152" s="12" t="s">
+      <c r="D152" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E152" t="s">
@@ -46698,7 +46703,7 @@
       <c r="C153" t="s">
         <v>40</v>
       </c>
-      <c r="D153" s="12">
+      <c r="D153" s="8">
         <v>71</v>
       </c>
       <c r="E153" t="s">
@@ -46715,7 +46720,7 @@
       <c r="C154" t="s">
         <v>40</v>
       </c>
-      <c r="D154" s="12">
+      <c r="D154" s="8">
         <v>70</v>
       </c>
       <c r="E154" t="s">
@@ -46732,7 +46737,7 @@
       <c r="C155" t="s">
         <v>40</v>
       </c>
-      <c r="D155" s="12">
+      <c r="D155" s="8">
         <v>69</v>
       </c>
       <c r="E155" t="s">
@@ -46749,7 +46754,7 @@
       <c r="C156" t="s">
         <v>40</v>
       </c>
-      <c r="D156" s="12">
+      <c r="D156" s="8">
         <v>66</v>
       </c>
       <c r="E156" t="s">
@@ -46766,7 +46771,7 @@
       <c r="C157" t="s">
         <v>40</v>
       </c>
-      <c r="D157" s="12">
+      <c r="D157" s="8">
         <v>62</v>
       </c>
       <c r="E157" t="s">
@@ -46783,7 +46788,7 @@
       <c r="C158" t="s">
         <v>40</v>
       </c>
-      <c r="D158" s="12">
+      <c r="D158" s="8">
         <v>61</v>
       </c>
       <c r="E158" t="s">
@@ -46800,7 +46805,7 @@
       <c r="C159" t="s">
         <v>40</v>
       </c>
-      <c r="D159" s="12">
+      <c r="D159" s="8">
         <v>60</v>
       </c>
       <c r="E159" t="s">
@@ -46817,7 +46822,7 @@
       <c r="C160" t="s">
         <v>40</v>
       </c>
-      <c r="D160" s="12">
+      <c r="D160" s="8">
         <v>56</v>
       </c>
       <c r="E160" t="s">
@@ -46834,7 +46839,7 @@
       <c r="C161" t="s">
         <v>40</v>
       </c>
-      <c r="D161" s="12">
+      <c r="D161" s="8">
         <v>52</v>
       </c>
       <c r="E161" t="s">
@@ -46851,7 +46856,7 @@
       <c r="C162" t="s">
         <v>40</v>
       </c>
-      <c r="D162" s="12">
+      <c r="D162" s="8">
         <v>50</v>
       </c>
       <c r="E162" t="s">
@@ -46868,7 +46873,7 @@
       <c r="C163" t="s">
         <v>40</v>
       </c>
-      <c r="D163" s="12">
+      <c r="D163" s="8">
         <v>49</v>
       </c>
       <c r="E163" t="s">
@@ -46885,7 +46890,7 @@
       <c r="C164" t="s">
         <v>40</v>
       </c>
-      <c r="D164" s="12">
+      <c r="D164" s="8">
         <v>47</v>
       </c>
       <c r="E164" t="s">
@@ -46902,7 +46907,7 @@
       <c r="C165" t="s">
         <v>40</v>
       </c>
-      <c r="D165" s="12">
+      <c r="D165" s="8">
         <v>39</v>
       </c>
       <c r="E165" t="s">
@@ -46919,7 +46924,7 @@
       <c r="C166" t="s">
         <v>40</v>
       </c>
-      <c r="D166" s="12">
+      <c r="D166" s="8">
         <v>38</v>
       </c>
       <c r="E166" t="s">
@@ -46936,7 +46941,7 @@
       <c r="C167" t="s">
         <v>40</v>
       </c>
-      <c r="D167" s="12">
+      <c r="D167" s="8">
         <v>35</v>
       </c>
       <c r="E167" t="s">
@@ -46953,7 +46958,7 @@
       <c r="C168" t="s">
         <v>40</v>
       </c>
-      <c r="D168" s="12">
+      <c r="D168" s="8">
         <v>30</v>
       </c>
       <c r="E168" t="s">
@@ -46970,7 +46975,7 @@
       <c r="C169" t="s">
         <v>40</v>
       </c>
-      <c r="D169" s="12">
+      <c r="D169" s="8">
         <v>29</v>
       </c>
       <c r="E169" t="s">
@@ -46987,7 +46992,7 @@
       <c r="C170" t="s">
         <v>40</v>
       </c>
-      <c r="D170" s="12">
+      <c r="D170" s="8">
         <v>28</v>
       </c>
       <c r="E170" t="s">
@@ -47004,7 +47009,7 @@
       <c r="C171" t="s">
         <v>40</v>
       </c>
-      <c r="D171" s="12">
+      <c r="D171" s="8">
         <v>25</v>
       </c>
       <c r="E171" t="s">
@@ -47021,7 +47026,7 @@
       <c r="C172" t="s">
         <v>40</v>
       </c>
-      <c r="D172" s="12">
+      <c r="D172" s="8">
         <v>24</v>
       </c>
       <c r="E172" t="s">
@@ -47038,7 +47043,7 @@
       <c r="C173" t="s">
         <v>40</v>
       </c>
-      <c r="D173" s="12">
+      <c r="D173" s="8">
         <v>23</v>
       </c>
       <c r="E173" t="s">
@@ -47055,7 +47060,7 @@
       <c r="C174" t="s">
         <v>40</v>
       </c>
-      <c r="D174" s="12">
+      <c r="D174" s="8">
         <v>21</v>
       </c>
       <c r="E174" t="s">
@@ -47072,7 +47077,7 @@
       <c r="C175" t="s">
         <v>40</v>
       </c>
-      <c r="D175" s="12">
+      <c r="D175" s="8">
         <v>20</v>
       </c>
       <c r="E175" t="s">
@@ -47089,7 +47094,7 @@
       <c r="C176" t="s">
         <v>40</v>
       </c>
-      <c r="D176" s="12">
+      <c r="D176" s="8">
         <v>19</v>
       </c>
       <c r="E176" t="s">
@@ -47106,7 +47111,7 @@
       <c r="C177" t="s">
         <v>40</v>
       </c>
-      <c r="D177" s="12">
+      <c r="D177" s="8">
         <v>15</v>
       </c>
       <c r="E177" t="s">
@@ -47123,7 +47128,7 @@
       <c r="C178" t="s">
         <v>40</v>
       </c>
-      <c r="D178" s="12">
+      <c r="D178" s="8">
         <v>12</v>
       </c>
       <c r="E178" t="s">
@@ -47140,7 +47145,7 @@
       <c r="C179" t="s">
         <v>40</v>
       </c>
-      <c r="D179" s="12">
+      <c r="D179" s="8">
         <v>11</v>
       </c>
       <c r="E179" t="s">
@@ -47157,7 +47162,7 @@
       <c r="C180" t="s">
         <v>40</v>
       </c>
-      <c r="D180" s="12">
+      <c r="D180" s="8">
         <v>8</v>
       </c>
       <c r="E180" t="s">
@@ -47174,7 +47179,7 @@
       <c r="C181" t="s">
         <v>40</v>
       </c>
-      <c r="D181" s="12">
+      <c r="D181" s="8">
         <v>6</v>
       </c>
       <c r="E181" t="s">
@@ -47191,7 +47196,7 @@
       <c r="C182" t="s">
         <v>40</v>
       </c>
-      <c r="D182" s="12">
+      <c r="D182" s="8">
         <v>5</v>
       </c>
       <c r="E182" t="s">
@@ -47208,7 +47213,7 @@
       <c r="C183" t="s">
         <v>40</v>
       </c>
-      <c r="D183" s="12">
+      <c r="D183" s="8">
         <v>3</v>
       </c>
       <c r="E183" t="s">
@@ -47225,7 +47230,7 @@
       <c r="C184" t="s">
         <v>48</v>
       </c>
-      <c r="D184" s="12">
+      <c r="D184" s="8">
         <v>146</v>
       </c>
       <c r="E184" t="s">
@@ -47242,7 +47247,7 @@
       <c r="C185" t="s">
         <v>48</v>
       </c>
-      <c r="D185" s="12">
+      <c r="D185" s="8">
         <v>138</v>
       </c>
       <c r="E185" t="s">
@@ -47259,7 +47264,7 @@
       <c r="C186" t="s">
         <v>48</v>
       </c>
-      <c r="D186" s="12">
+      <c r="D186" s="8">
         <v>137</v>
       </c>
       <c r="E186" t="s">
@@ -47276,7 +47281,7 @@
       <c r="C187" t="s">
         <v>48</v>
       </c>
-      <c r="D187" s="12">
+      <c r="D187" s="8">
         <v>130</v>
       </c>
       <c r="E187" t="s">
@@ -47293,7 +47298,7 @@
       <c r="C188" t="s">
         <v>48</v>
       </c>
-      <c r="D188" s="12">
+      <c r="D188" s="8">
         <v>127</v>
       </c>
       <c r="E188" t="s">
@@ -47310,7 +47315,7 @@
       <c r="C189" t="s">
         <v>48</v>
       </c>
-      <c r="D189" s="12">
+      <c r="D189" s="8">
         <v>120</v>
       </c>
       <c r="E189" t="s">
@@ -47327,7 +47332,7 @@
       <c r="C190" t="s">
         <v>48</v>
       </c>
-      <c r="D190" s="12">
+      <c r="D190" s="8">
         <v>113</v>
       </c>
       <c r="E190" t="s">
@@ -47344,7 +47349,7 @@
       <c r="C191" t="s">
         <v>48</v>
       </c>
-      <c r="D191" s="12">
+      <c r="D191" s="8">
         <v>111</v>
       </c>
       <c r="E191" t="s">
@@ -47361,7 +47366,7 @@
       <c r="C192" t="s">
         <v>48</v>
       </c>
-      <c r="D192" s="12">
+      <c r="D192" s="8">
         <v>108</v>
       </c>
       <c r="E192" t="s">
@@ -47378,7 +47383,7 @@
       <c r="C193" t="s">
         <v>48</v>
       </c>
-      <c r="D193" s="12">
+      <c r="D193" s="8">
         <v>99</v>
       </c>
       <c r="E193" t="s">
@@ -47395,7 +47400,7 @@
       <c r="C194" t="s">
         <v>48</v>
       </c>
-      <c r="D194" s="12">
+      <c r="D194" s="8">
         <v>98</v>
       </c>
       <c r="E194" t="s">
@@ -47412,7 +47417,7 @@
       <c r="C195" t="s">
         <v>48</v>
       </c>
-      <c r="D195" s="12">
+      <c r="D195" s="8">
         <v>94</v>
       </c>
       <c r="E195" t="s">
@@ -47429,7 +47434,7 @@
       <c r="C196" t="s">
         <v>48</v>
       </c>
-      <c r="D196" s="12">
+      <c r="D196" s="8">
         <v>92</v>
       </c>
       <c r="E196" t="s">
@@ -47446,7 +47451,7 @@
       <c r="C197" t="s">
         <v>48</v>
       </c>
-      <c r="D197" s="12">
+      <c r="D197" s="8">
         <v>85</v>
       </c>
       <c r="E197" t="s">
@@ -47463,7 +47468,7 @@
       <c r="C198" t="s">
         <v>48</v>
       </c>
-      <c r="D198" s="12">
+      <c r="D198" s="8">
         <v>81</v>
       </c>
       <c r="E198" t="s">
@@ -47480,7 +47485,7 @@
       <c r="C199" t="s">
         <v>48</v>
       </c>
-      <c r="D199" s="12">
+      <c r="D199" s="8">
         <v>75</v>
       </c>
       <c r="E199" t="s">
@@ -47497,7 +47502,7 @@
       <c r="C200" t="s">
         <v>48</v>
       </c>
-      <c r="D200" s="12">
+      <c r="D200" s="8">
         <v>70</v>
       </c>
       <c r="E200" t="s">
@@ -47514,14 +47519,14 @@
       <c r="C201" t="s">
         <v>48</v>
       </c>
-      <c r="D201" s="12">
+      <c r="D201" s="8">
         <v>68</v>
       </c>
       <c r="E201" t="s">
         <v>37</v>
       </c>
       <c r="F201" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.3">
@@ -47534,7 +47539,7 @@
       <c r="C202" t="s">
         <v>48</v>
       </c>
-      <c r="D202" s="12">
+      <c r="D202" s="8">
         <v>67</v>
       </c>
       <c r="E202" t="s">
@@ -47551,7 +47556,7 @@
       <c r="C203" t="s">
         <v>48</v>
       </c>
-      <c r="D203" s="12">
+      <c r="D203" s="8">
         <v>64</v>
       </c>
       <c r="E203" t="s">
@@ -47568,7 +47573,7 @@
       <c r="C204" t="s">
         <v>48</v>
       </c>
-      <c r="D204" s="12">
+      <c r="D204" s="8">
         <v>60</v>
       </c>
       <c r="E204" t="s">
@@ -47585,7 +47590,7 @@
       <c r="C205" t="s">
         <v>48</v>
       </c>
-      <c r="D205" s="12">
+      <c r="D205" s="8">
         <v>56</v>
       </c>
       <c r="E205" t="s">
@@ -47602,7 +47607,7 @@
       <c r="C206" t="s">
         <v>48</v>
       </c>
-      <c r="D206" s="12">
+      <c r="D206" s="8">
         <v>53</v>
       </c>
       <c r="E206" t="s">
@@ -47619,7 +47624,7 @@
       <c r="C207" t="s">
         <v>48</v>
       </c>
-      <c r="D207" s="12">
+      <c r="D207" s="8">
         <v>52</v>
       </c>
       <c r="E207" t="s">
@@ -47636,7 +47641,7 @@
       <c r="C208" t="s">
         <v>48</v>
       </c>
-      <c r="D208" s="12">
+      <c r="D208" s="8">
         <v>50</v>
       </c>
       <c r="E208" t="s">
@@ -47653,7 +47658,7 @@
       <c r="C209" t="s">
         <v>48</v>
       </c>
-      <c r="D209" s="12">
+      <c r="D209" s="8">
         <v>49</v>
       </c>
       <c r="E209" t="s">
@@ -47670,7 +47675,7 @@
       <c r="C210" t="s">
         <v>48</v>
       </c>
-      <c r="D210" s="12">
+      <c r="D210" s="8">
         <v>47</v>
       </c>
       <c r="E210" t="s">
@@ -47687,7 +47692,7 @@
       <c r="C211" t="s">
         <v>48</v>
       </c>
-      <c r="D211" s="12">
+      <c r="D211" s="8">
         <v>35</v>
       </c>
       <c r="E211" t="s">
@@ -47704,7 +47709,7 @@
       <c r="C212" t="s">
         <v>48</v>
       </c>
-      <c r="D212" s="12">
+      <c r="D212" s="8">
         <v>33</v>
       </c>
       <c r="E212" t="s">
@@ -47721,7 +47726,7 @@
       <c r="C213" t="s">
         <v>48</v>
       </c>
-      <c r="D213" s="12">
+      <c r="D213" s="8">
         <v>30</v>
       </c>
       <c r="E213" t="s">
@@ -47738,7 +47743,7 @@
       <c r="C214" t="s">
         <v>48</v>
       </c>
-      <c r="D214" s="12">
+      <c r="D214" s="8">
         <v>26</v>
       </c>
       <c r="E214" t="s">
@@ -47755,7 +47760,7 @@
       <c r="C215" t="s">
         <v>48</v>
       </c>
-      <c r="D215" s="12">
+      <c r="D215" s="8">
         <v>25</v>
       </c>
       <c r="E215" t="s">
@@ -47772,14 +47777,14 @@
       <c r="C216" t="s">
         <v>48</v>
       </c>
-      <c r="D216" s="12">
+      <c r="D216" s="8">
         <v>14</v>
       </c>
       <c r="E216" t="s">
         <v>23</v>
       </c>
       <c r="F216" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.3">
@@ -47792,7 +47797,7 @@
       <c r="C217" t="s">
         <v>48</v>
       </c>
-      <c r="D217" s="12">
+      <c r="D217" s="8">
         <v>8</v>
       </c>
       <c r="E217" t="s">
@@ -47812,7 +47817,7 @@
       <c r="C218" t="s">
         <v>48</v>
       </c>
-      <c r="D218" s="12">
+      <c r="D218" s="8">
         <v>5</v>
       </c>
       <c r="E218" t="s">
@@ -47829,7 +47834,7 @@
       <c r="C219" t="s">
         <v>48</v>
       </c>
-      <c r="D219" s="12">
+      <c r="D219" s="8">
         <v>4</v>
       </c>
       <c r="E219" t="s">
@@ -47846,7 +47851,7 @@
       <c r="C220" t="s">
         <v>49</v>
       </c>
-      <c r="D220" s="12">
+      <c r="D220" s="8">
         <v>146</v>
       </c>
       <c r="E220" t="s">
@@ -47863,7 +47868,7 @@
       <c r="C221" t="s">
         <v>49</v>
       </c>
-      <c r="D221" s="12">
+      <c r="D221" s="8">
         <v>140</v>
       </c>
       <c r="E221" t="s">
@@ -47880,7 +47885,7 @@
       <c r="C222" t="s">
         <v>49</v>
       </c>
-      <c r="D222" s="12">
+      <c r="D222" s="8">
         <v>134</v>
       </c>
       <c r="E222" t="s">
@@ -47897,7 +47902,7 @@
       <c r="C223" t="s">
         <v>49</v>
       </c>
-      <c r="D223" s="12">
+      <c r="D223" s="8">
         <v>122</v>
       </c>
       <c r="E223" t="s">
@@ -47914,7 +47919,7 @@
       <c r="C224" t="s">
         <v>49</v>
       </c>
-      <c r="D224" s="12">
+      <c r="D224" s="8">
         <v>90</v>
       </c>
       <c r="E224" t="s">
@@ -47931,7 +47936,7 @@
       <c r="C225" t="s">
         <v>49</v>
       </c>
-      <c r="D225" s="12">
+      <c r="D225" s="8">
         <v>85</v>
       </c>
       <c r="E225" t="s">
@@ -47948,7 +47953,7 @@
       <c r="C226" t="s">
         <v>49</v>
       </c>
-      <c r="D226" s="12">
+      <c r="D226" s="8">
         <v>87</v>
       </c>
       <c r="E226" t="s">
@@ -47965,7 +47970,7 @@
       <c r="C227" t="s">
         <v>49</v>
       </c>
-      <c r="D227" s="12">
+      <c r="D227" s="8">
         <v>83</v>
       </c>
       <c r="E227" t="s">
@@ -47982,7 +47987,7 @@
       <c r="C228" t="s">
         <v>49</v>
       </c>
-      <c r="D228" s="12">
+      <c r="D228" s="8">
         <v>81</v>
       </c>
       <c r="E228" t="s">
@@ -47999,7 +48004,7 @@
       <c r="C229" t="s">
         <v>49</v>
       </c>
-      <c r="D229" s="12">
+      <c r="D229" s="8">
         <v>74</v>
       </c>
       <c r="E229" t="s">
@@ -48016,7 +48021,7 @@
       <c r="C230" t="s">
         <v>49</v>
       </c>
-      <c r="D230" s="12">
+      <c r="D230" s="8">
         <v>50</v>
       </c>
       <c r="E230" t="s">
@@ -48033,7 +48038,7 @@
       <c r="C231" t="s">
         <v>49</v>
       </c>
-      <c r="D231" s="12">
+      <c r="D231" s="8">
         <v>49</v>
       </c>
       <c r="E231" t="s">
@@ -48050,7 +48055,7 @@
       <c r="C232" t="s">
         <v>49</v>
       </c>
-      <c r="D232" s="12">
+      <c r="D232" s="8">
         <v>35</v>
       </c>
       <c r="E232" t="s">
@@ -48067,7 +48072,7 @@
       <c r="C233" t="s">
         <v>49</v>
       </c>
-      <c r="D233" s="12">
+      <c r="D233" s="8">
         <v>28</v>
       </c>
       <c r="E233" t="s">
@@ -48084,7 +48089,7 @@
       <c r="C234" t="s">
         <v>49</v>
       </c>
-      <c r="D234" s="12">
+      <c r="D234" s="8">
         <v>25</v>
       </c>
       <c r="E234" t="s">
@@ -48101,7 +48106,7 @@
       <c r="C235" t="s">
         <v>49</v>
       </c>
-      <c r="D235" s="12">
+      <c r="D235" s="8">
         <v>13</v>
       </c>
       <c r="E235" t="s">
@@ -48118,7 +48123,7 @@
       <c r="C236" t="s">
         <v>49</v>
       </c>
-      <c r="D236" s="12">
+      <c r="D236" s="8">
         <v>10</v>
       </c>
       <c r="E236" t="s">
@@ -48135,7 +48140,7 @@
       <c r="C237" t="s">
         <v>49</v>
       </c>
-      <c r="D237" s="12">
+      <c r="D237" s="8">
         <v>8</v>
       </c>
       <c r="E237" t="s">
@@ -48152,7 +48157,7 @@
       <c r="C238" t="s">
         <v>49</v>
       </c>
-      <c r="D238" s="12">
+      <c r="D238" s="8">
         <v>1</v>
       </c>
       <c r="E238" t="s">
@@ -48169,7 +48174,7 @@
       <c r="C239" t="s">
         <v>53</v>
       </c>
-      <c r="D239" s="12">
+      <c r="D239" s="8">
         <v>149</v>
       </c>
       <c r="E239" t="s">
@@ -48186,7 +48191,7 @@
       <c r="C240" t="s">
         <v>53</v>
       </c>
-      <c r="D240" s="12">
+      <c r="D240" s="8">
         <v>145</v>
       </c>
       <c r="E240" t="s">
@@ -48203,7 +48208,7 @@
       <c r="C241" t="s">
         <v>53</v>
       </c>
-      <c r="D241" s="12">
+      <c r="D241" s="8">
         <v>140</v>
       </c>
       <c r="E241" t="s">
@@ -48220,7 +48225,7 @@
       <c r="C242" t="s">
         <v>53</v>
       </c>
-      <c r="D242" s="12">
+      <c r="D242" s="8">
         <v>139</v>
       </c>
       <c r="E242" t="s">
@@ -48237,7 +48242,7 @@
       <c r="C243" t="s">
         <v>53</v>
       </c>
-      <c r="D243" s="12">
+      <c r="D243" s="8">
         <v>138</v>
       </c>
       <c r="E243" t="s">
@@ -48254,7 +48259,7 @@
       <c r="C244" t="s">
         <v>53</v>
       </c>
-      <c r="D244" s="12">
+      <c r="D244" s="8">
         <v>136</v>
       </c>
       <c r="E244" t="s">
@@ -48271,7 +48276,7 @@
       <c r="C245" t="s">
         <v>53</v>
       </c>
-      <c r="D245" s="12">
+      <c r="D245" s="8">
         <v>132</v>
       </c>
       <c r="E245" t="s">
@@ -48288,7 +48293,7 @@
       <c r="C246" t="s">
         <v>53</v>
       </c>
-      <c r="D246" s="12">
+      <c r="D246" s="8">
         <v>123</v>
       </c>
       <c r="E246" t="s">
@@ -48305,7 +48310,7 @@
       <c r="C247" t="s">
         <v>53</v>
       </c>
-      <c r="D247" s="12">
+      <c r="D247" s="8">
         <v>114</v>
       </c>
       <c r="E247" t="s">
@@ -48322,7 +48327,7 @@
       <c r="C248" t="s">
         <v>53</v>
       </c>
-      <c r="D248" s="12">
+      <c r="D248" s="8">
         <v>109</v>
       </c>
       <c r="E248" t="s">
@@ -48339,7 +48344,7 @@
       <c r="C249" t="s">
         <v>53</v>
       </c>
-      <c r="D249" s="12">
+      <c r="D249" s="8">
         <v>108</v>
       </c>
       <c r="E249" t="s">
@@ -48356,7 +48361,7 @@
       <c r="C250" t="s">
         <v>53</v>
       </c>
-      <c r="D250" s="12">
+      <c r="D250" s="8">
         <v>104</v>
       </c>
       <c r="E250" t="s">
@@ -48373,7 +48378,7 @@
       <c r="C251" t="s">
         <v>53</v>
       </c>
-      <c r="D251" s="12">
+      <c r="D251" s="8">
         <v>103</v>
       </c>
       <c r="E251" t="s">
@@ -48390,7 +48395,7 @@
       <c r="C252" t="s">
         <v>53</v>
       </c>
-      <c r="D252" s="12">
+      <c r="D252" s="8">
         <v>102</v>
       </c>
       <c r="E252" t="s">
@@ -48407,7 +48412,7 @@
       <c r="C253" t="s">
         <v>53</v>
       </c>
-      <c r="D253" s="12">
+      <c r="D253" s="8">
         <v>85</v>
       </c>
       <c r="E253" t="s">
@@ -48424,7 +48429,7 @@
       <c r="C254" t="s">
         <v>53</v>
       </c>
-      <c r="D254" s="12" t="s">
+      <c r="D254" s="8" t="s">
         <v>58</v>
       </c>
       <c r="E254" t="s">
@@ -48441,7 +48446,7 @@
       <c r="C255" t="s">
         <v>53</v>
       </c>
-      <c r="D255" s="12" t="s">
+      <c r="D255" s="8" t="s">
         <v>59</v>
       </c>
       <c r="E255" t="s">
@@ -48458,7 +48463,7 @@
       <c r="C256" t="s">
         <v>53</v>
       </c>
-      <c r="D256" s="12">
+      <c r="D256" s="8">
         <v>80</v>
       </c>
       <c r="E256" t="s">
@@ -48475,7 +48480,7 @@
       <c r="C257" t="s">
         <v>53</v>
       </c>
-      <c r="D257" s="12">
+      <c r="D257" s="8">
         <v>75</v>
       </c>
       <c r="E257" t="s">
@@ -48492,7 +48497,7 @@
       <c r="C258" t="s">
         <v>53</v>
       </c>
-      <c r="D258" s="12">
+      <c r="D258" s="8">
         <v>70</v>
       </c>
       <c r="E258" t="s">
@@ -48509,7 +48514,7 @@
       <c r="C259" t="s">
         <v>53</v>
       </c>
-      <c r="D259" s="12">
+      <c r="D259" s="8">
         <v>68</v>
       </c>
       <c r="E259" t="s">
@@ -48526,7 +48531,7 @@
       <c r="C260" t="s">
         <v>53</v>
       </c>
-      <c r="D260" s="12">
+      <c r="D260" s="8">
         <v>61</v>
       </c>
       <c r="E260" t="s">
@@ -48543,7 +48548,7 @@
       <c r="C261" t="s">
         <v>53</v>
       </c>
-      <c r="D261" s="12">
+      <c r="D261" s="8">
         <v>55</v>
       </c>
       <c r="E261" t="s">
@@ -48560,7 +48565,7 @@
       <c r="C262" t="s">
         <v>53</v>
       </c>
-      <c r="D262" s="12">
+      <c r="D262" s="8">
         <v>50</v>
       </c>
       <c r="E262" t="s">
@@ -48577,7 +48582,7 @@
       <c r="C263" t="s">
         <v>53</v>
       </c>
-      <c r="D263" s="12">
+      <c r="D263" s="8">
         <v>42</v>
       </c>
       <c r="E263" t="s">
@@ -48594,7 +48599,7 @@
       <c r="C264" t="s">
         <v>53</v>
       </c>
-      <c r="D264" s="12">
+      <c r="D264" s="8">
         <v>40</v>
       </c>
       <c r="E264" t="s">
@@ -48611,7 +48616,7 @@
       <c r="C265" t="s">
         <v>53</v>
       </c>
-      <c r="D265" s="12">
+      <c r="D265" s="8">
         <v>38</v>
       </c>
       <c r="E265" t="s">
@@ -48628,7 +48633,7 @@
       <c r="C266" t="s">
         <v>53</v>
       </c>
-      <c r="D266" s="12">
+      <c r="D266" s="8">
         <v>36</v>
       </c>
       <c r="E266" t="s">
@@ -48645,7 +48650,7 @@
       <c r="C267" t="s">
         <v>53</v>
       </c>
-      <c r="D267" s="12">
+      <c r="D267" s="8">
         <v>35</v>
       </c>
       <c r="E267" t="s">
@@ -48662,7 +48667,7 @@
       <c r="C268" t="s">
         <v>53</v>
       </c>
-      <c r="D268" s="12">
+      <c r="D268" s="8">
         <v>33</v>
       </c>
       <c r="E268" t="s">
@@ -48679,7 +48684,7 @@
       <c r="C269" t="s">
         <v>53</v>
       </c>
-      <c r="D269" s="12">
+      <c r="D269" s="8">
         <v>26</v>
       </c>
       <c r="E269" t="s">
@@ -48696,7 +48701,7 @@
       <c r="C270" t="s">
         <v>53</v>
       </c>
-      <c r="D270" s="12">
+      <c r="D270" s="8">
         <v>23</v>
       </c>
       <c r="E270" t="s">
@@ -48713,7 +48718,7 @@
       <c r="C271" t="s">
         <v>53</v>
       </c>
-      <c r="D271" s="12">
+      <c r="D271" s="8">
         <v>22</v>
       </c>
       <c r="E271" t="s">
@@ -48730,7 +48735,7 @@
       <c r="C272" t="s">
         <v>53</v>
       </c>
-      <c r="D272" s="12">
+      <c r="D272" s="8">
         <v>21</v>
       </c>
       <c r="E272" t="s">
@@ -48747,7 +48752,7 @@
       <c r="C273" t="s">
         <v>53</v>
       </c>
-      <c r="D273" s="12">
+      <c r="D273" s="8">
         <v>13</v>
       </c>
       <c r="E273" t="s">
@@ -48764,7 +48769,7 @@
       <c r="C274" t="s">
         <v>53</v>
       </c>
-      <c r="D274" s="12">
+      <c r="D274" s="8">
         <v>12</v>
       </c>
       <c r="E274" t="s">
@@ -48781,7 +48786,7 @@
       <c r="C275" t="s">
         <v>53</v>
       </c>
-      <c r="D275" s="12">
+      <c r="D275" s="8">
         <v>11</v>
       </c>
       <c r="E275" t="s">
@@ -48798,7 +48803,7 @@
       <c r="C276" t="s">
         <v>53</v>
       </c>
-      <c r="D276" s="12">
+      <c r="D276" s="8">
         <v>1</v>
       </c>
       <c r="E276" t="s">
@@ -48815,7 +48820,7 @@
       <c r="C277" t="s">
         <v>61</v>
       </c>
-      <c r="D277" s="12">
+      <c r="D277" s="8">
         <v>144</v>
       </c>
       <c r="E277" t="s">
@@ -48832,7 +48837,7 @@
       <c r="C278" t="s">
         <v>61</v>
       </c>
-      <c r="D278" s="12">
+      <c r="D278" s="8">
         <v>143</v>
       </c>
       <c r="E278" t="s">
@@ -48849,7 +48854,7 @@
       <c r="C279" t="s">
         <v>61</v>
       </c>
-      <c r="D279" s="12">
+      <c r="D279" s="8">
         <v>136</v>
       </c>
       <c r="E279" t="s">
@@ -48866,7 +48871,7 @@
       <c r="C280" t="s">
         <v>61</v>
       </c>
-      <c r="D280" s="12">
+      <c r="D280" s="8">
         <v>133</v>
       </c>
       <c r="E280" t="s">
@@ -48883,7 +48888,7 @@
       <c r="C281" t="s">
         <v>61</v>
       </c>
-      <c r="D281" s="12">
+      <c r="D281" s="8">
         <v>125</v>
       </c>
       <c r="E281" t="s">
@@ -48900,7 +48905,7 @@
       <c r="C282" t="s">
         <v>61</v>
       </c>
-      <c r="D282" s="12">
+      <c r="D282" s="8">
         <v>124</v>
       </c>
       <c r="E282" t="s">
@@ -48917,7 +48922,7 @@
       <c r="C283" t="s">
         <v>61</v>
       </c>
-      <c r="D283" s="12">
+      <c r="D283" s="8">
         <v>116</v>
       </c>
       <c r="E283" t="s">
@@ -48934,7 +48939,7 @@
       <c r="C284" t="s">
         <v>61</v>
       </c>
-      <c r="D284" s="12">
+      <c r="D284" s="8">
         <v>104</v>
       </c>
       <c r="E284" t="s">
@@ -48951,7 +48956,7 @@
       <c r="C285" t="s">
         <v>61</v>
       </c>
-      <c r="D285" s="12">
+      <c r="D285" s="8">
         <v>81</v>
       </c>
       <c r="E285" t="s">
@@ -48968,7 +48973,7 @@
       <c r="C286" t="s">
         <v>61</v>
       </c>
-      <c r="D286" s="12">
+      <c r="D286" s="8">
         <v>79</v>
       </c>
       <c r="E286" t="s">
@@ -48985,7 +48990,7 @@
       <c r="C287" t="s">
         <v>61</v>
       </c>
-      <c r="D287" s="12">
+      <c r="D287" s="8">
         <v>77</v>
       </c>
       <c r="E287" t="s">
@@ -49002,7 +49007,7 @@
       <c r="C288" t="s">
         <v>61</v>
       </c>
-      <c r="D288" s="12">
+      <c r="D288" s="8">
         <v>43</v>
       </c>
       <c r="E288" t="s">
@@ -49019,7 +49024,7 @@
       <c r="C289" t="s">
         <v>61</v>
       </c>
-      <c r="D289" s="12">
+      <c r="D289" s="8">
         <v>39</v>
       </c>
       <c r="E289" t="s">
@@ -49036,7 +49041,7 @@
       <c r="C290" t="s">
         <v>61</v>
       </c>
-      <c r="D290" s="12">
+      <c r="D290" s="8">
         <v>29</v>
       </c>
       <c r="E290" t="s">
@@ -49053,7 +49058,7 @@
       <c r="C291" t="s">
         <v>61</v>
       </c>
-      <c r="D291" s="12">
+      <c r="D291" s="8">
         <v>19</v>
       </c>
       <c r="E291" t="s">
@@ -49070,7 +49075,7 @@
       <c r="C292" t="s">
         <v>61</v>
       </c>
-      <c r="D292" s="12">
+      <c r="D292" s="8">
         <v>16</v>
       </c>
       <c r="E292" t="s">
@@ -49087,7 +49092,7 @@
       <c r="C293" t="s">
         <v>61</v>
       </c>
-      <c r="D293" s="12">
+      <c r="D293" s="8">
         <v>9</v>
       </c>
       <c r="E293" t="s">
@@ -49104,7 +49109,7 @@
       <c r="C294" t="s">
         <v>61</v>
       </c>
-      <c r="D294" s="12">
+      <c r="D294" s="8">
         <v>4</v>
       </c>
       <c r="E294" t="s">
@@ -49121,7 +49126,7 @@
       <c r="C295" t="s">
         <v>61</v>
       </c>
-      <c r="D295" s="12">
+      <c r="D295" s="8">
         <v>2</v>
       </c>
       <c r="E295" t="s">
@@ -49144,7 +49149,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -49153,315 +49158,320 @@
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
     </row>
     <row r="2" spans="1:15" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
+      <c r="A2" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="B3" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>174</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H8" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" t="s">
-        <v>168</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" t="s">
         <v>167</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I9" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
         <v>166</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>7</v>
+      <c r="H10" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="I10" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>159</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>30</v>
+        <v>165</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="I11" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>165</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>14</v>
+        <v>158</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="I12" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
         <v>164</v>
       </c>
-      <c r="H13" t="s">
-        <v>17</v>
+      <c r="H13" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="I13" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
         <v>163</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>37</v>
+      <c r="H14" t="s">
+        <v>17</v>
       </c>
       <c r="I14" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
         <v>162</v>
       </c>
-      <c r="H15" t="s">
-        <v>15</v>
+      <c r="H15" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="I15" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" t="s">
+        <v>161</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>97</v>
       </c>
-      <c r="B16" t="s">
-        <v>160</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="B17" t="s">
+        <v>159</v>
+      </c>
+      <c r="H17" t="s">
         <v>18</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I17" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H17" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
         <v>38</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H18" s="3" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I19" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="H19" t="s">
-        <v>41</v>
-      </c>
-      <c r="I19" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H21" t="s">
         <v>9</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I21" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" t="s">
-        <v>168</v>
-      </c>
-      <c r="H21" t="s">
-        <v>33</v>
-      </c>
-      <c r="I21" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="H22" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="I22" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="H23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I23" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I24" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>173</v>
+        <v>168</v>
+      </c>
+      <c r="H25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>151</v>
       </c>
-      <c r="B26" t="s">
-        <v>170</v>
+      <c r="B27" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>